<commit_message>
Vendor Pincode Mapping Table Cleaning- Changes in file download and upload(Vendor Mapping file)
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/vendor_pin_code.xlsx
+++ b/application/controllers/excel-templates/vendor_pin_code.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,32 +24,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>{order:Vendor_Name}</t>
   </si>
   <si>
-    <t>{order:Vendor_ID}</t>
-  </si>
-  <si>
     <t>{order:Appliance}</t>
   </si>
   <si>
-    <t>{order:Appliance_ID}</t>
-  </si>
-  <si>
-    <t>{order:Brand}</t>
-  </si>
-  <si>
-    <t>{order:Area}</t>
-  </si>
-  <si>
     <t>{order:Pincode}</t>
   </si>
   <si>
-    <t>{order:Region}</t>
-  </si>
-  <si>
     <t>{order:City}</t>
   </si>
   <si>
@@ -59,25 +44,10 @@
     <t>vendor_name</t>
   </si>
   <si>
-    <t>vendor_id</t>
-  </si>
-  <si>
     <t>appliance</t>
   </si>
   <si>
-    <t>appliance_id</t>
-  </si>
-  <si>
-    <t>brand</t>
-  </si>
-  <si>
-    <t>area</t>
-  </si>
-  <si>
     <t>pincode</t>
-  </si>
-  <si>
-    <t>region</t>
   </si>
   <si>
     <t>city</t>
@@ -152,7 +122,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office विषयवस्तु">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -448,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{694C6217-1555-414E-9DEF-C07118457997}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,39 +429,24 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -506,21 +461,6 @@
       </c>
       <c r="E2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change Notification Center Color For Partner and in partner login take public name instead of name
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/vendor_pin_code.xlsx
+++ b/application/controllers/excel-templates/vendor_pin_code.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>{order:Vendor_Name}</t>
   </si>
@@ -35,12 +35,6 @@
     <t>{order:Pincode}</t>
   </si>
   <si>
-    <t>{order:City}</t>
-  </si>
-  <si>
-    <t>{order:State}</t>
-  </si>
-  <si>
     <t>vendor_name</t>
   </si>
   <si>
@@ -48,12 +42,6 @@
   </si>
   <si>
     <t>pincode</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>state</t>
   </si>
 </sst>
 </file>
@@ -418,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{694C6217-1555-414E-9DEF-C07118457997}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,24 +417,18 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -455,12 +437,6 @@
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>